<commit_message>
rename Obs slots and rebuild Data objects
</commit_message>
<xml_diff>
--- a/inst/Example_Chile_Hake.xlsx
+++ b/inst/Example_Chile_Hake.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Dropbox\Projects\DLMtoolDev\OM_doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Documents\GitHub\DLMtool\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8970" tabRatio="736" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8970" tabRatio="736" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OM" sheetId="13" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="106">
   <si>
     <t>Name</t>
   </si>
@@ -199,63 +199,9 @@
     <t>Iobs</t>
   </si>
   <si>
-    <t>Mcv</t>
-  </si>
-  <si>
-    <t>Kcv</t>
-  </si>
-  <si>
-    <t>t0cv</t>
-  </si>
-  <si>
-    <t>Linfcv</t>
-  </si>
-  <si>
-    <t>LFCcv</t>
-  </si>
-  <si>
-    <t>LFScv</t>
-  </si>
-  <si>
-    <t>FMSYcv</t>
-  </si>
-  <si>
-    <t>FMSY_Mcv</t>
-  </si>
-  <si>
-    <t>BMSY_B0cv</t>
-  </si>
-  <si>
     <t>Dbiascv</t>
   </si>
   <si>
-    <t>Dcv</t>
-  </si>
-  <si>
-    <t>Btbias</t>
-  </si>
-  <si>
-    <t>Btcv</t>
-  </si>
-  <si>
-    <t>hcv</t>
-  </si>
-  <si>
-    <t>Icv</t>
-  </si>
-  <si>
-    <t>Reccv</t>
-  </si>
-  <si>
-    <t>Irefcv</t>
-  </si>
-  <si>
-    <t>Crefcv</t>
-  </si>
-  <si>
-    <t>Brefcv</t>
-  </si>
-  <si>
     <t>beta</t>
   </si>
   <si>
@@ -265,12 +211,6 @@
     <t>TACFrac</t>
   </si>
   <si>
-    <t>ESD</t>
-  </si>
-  <si>
-    <t>EFrac</t>
-  </si>
-  <si>
     <t>SizeLimSD</t>
   </si>
   <si>
@@ -319,24 +259,6 @@
     <t>Chile_hake</t>
   </si>
   <si>
-    <t>CALcv</t>
-  </si>
-  <si>
-    <t>B0cv</t>
-  </si>
-  <si>
-    <t>rcv</t>
-  </si>
-  <si>
-    <t>Fcurbiascv</t>
-  </si>
-  <si>
-    <t>Fcurcv</t>
-  </si>
-  <si>
-    <t>maxagecv</t>
-  </si>
-  <si>
     <t>Slot</t>
   </si>
   <si>
@@ -367,9 +289,6 @@
     <t>Mexp</t>
   </si>
   <si>
-    <t>recgrad</t>
-  </si>
-  <si>
     <t>LenCV</t>
   </si>
   <si>
@@ -383,13 +302,73 @@
   </si>
   <si>
     <t>Chilean hake stock assessment 2017</t>
+  </si>
+  <si>
+    <t>Btbiascv</t>
+  </si>
+  <si>
+    <t>Ibiascv</t>
+  </si>
+  <si>
+    <t>Dobs</t>
+  </si>
+  <si>
+    <t>Btobs</t>
+  </si>
+  <si>
+    <t>Mbiascv</t>
+  </si>
+  <si>
+    <t>Kbiascv</t>
+  </si>
+  <si>
+    <t>t0biascv</t>
+  </si>
+  <si>
+    <t>Linfbiascv</t>
+  </si>
+  <si>
+    <t>LFCbiascv</t>
+  </si>
+  <si>
+    <t>LFSbiascv</t>
+  </si>
+  <si>
+    <t>FMSYbiascv</t>
+  </si>
+  <si>
+    <t>FMSY_Mbiascv</t>
+  </si>
+  <si>
+    <t>BMSY_B0biascv</t>
+  </si>
+  <si>
+    <t>Irefbiascv</t>
+  </si>
+  <si>
+    <t>Crefbiascv</t>
+  </si>
+  <si>
+    <t>Brefbiascv</t>
+  </si>
+  <si>
+    <t>hbiascv</t>
+  </si>
+  <si>
+    <t>Recbiascv</t>
+  </si>
+  <si>
+    <t>TAESD</t>
+  </si>
+  <si>
+    <t>TAEFrac</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -405,6 +384,20 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -440,15 +433,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,7 +463,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6AE37E10-657C-4A4F-A847-0C0BD77C6FA9}" name="Table3" displayName="Table3" ref="A1:C33" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6AE37E10-657C-4A4F-A847-0C0BD77C6FA9}" name="Table3" displayName="Table3" ref="A1:C32" totalsRowShown="0">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{DADCC3AD-4B5F-4A7E-BD98-F7CBEA65EAB6}" name="Slot"/>
     <tableColumn id="2" xr3:uid="{FA5D409C-1457-4647-931B-71E61908547B}" name="Column1"/>
@@ -789,7 +784,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -797,12 +792,12 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="B3">
         <v>200</v>
@@ -810,7 +805,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="B4">
         <v>50</v>
@@ -818,7 +813,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -826,35 +821,35 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="B6">
         <v>0.5</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="B7">
         <v>0.8</v>
       </c>
       <c r="C7" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -864,10 +859,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,13 +874,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="B1" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="C1" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -895,7 +890,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -927,12 +922,12 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1006,161 +1001,168 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>107</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>69.27</v>
+      </c>
+      <c r="C16">
+        <v>78.099999999999994</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B17">
-        <v>69.27</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="C17">
-        <v>78.099999999999994</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B18">
-        <v>0.14000000000000001</v>
+        <v>-0.65700000000000003</v>
       </c>
       <c r="C18">
-        <v>0.2</v>
+        <v>-0.23200000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="B19">
-        <v>-0.65700000000000003</v>
+        <v>0.1</v>
       </c>
       <c r="C19">
-        <v>-0.23200000000000001</v>
-      </c>
+        <v>0.12</v>
+      </c>
+      <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="B20">
+        <v>0.05</v>
+      </c>
+      <c r="C20">
         <v>0.1</v>
       </c>
-      <c r="C20">
-        <v>0.12</v>
-      </c>
-      <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B21">
-        <v>0.05</v>
+        <v>-0.01</v>
       </c>
       <c r="C21">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B22">
-        <v>-0.01</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="C22">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B23">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="C23">
-        <v>0.05</v>
+        <v>-0.01</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.01</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B24">
-        <v>-0.01</v>
-      </c>
-      <c r="C24" s="2">
-        <v>0.01</v>
+        <v>36</v>
+      </c>
+      <c r="C24">
+        <v>37.4</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B25">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="C25">
-        <v>37.4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B26">
-        <v>5</v>
+        <v>0.15</v>
       </c>
       <c r="C26">
-        <v>10</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B27">
-        <v>0.15</v>
-      </c>
-      <c r="C27">
-        <v>0.25</v>
+        <v>1.5999999999999999E-5</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B28">
-        <v>1.5999999999999999E-5</v>
-      </c>
+        <v>2.77</v>
+      </c>
+      <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B29">
-        <v>2.77</v>
+        <v>0.5</v>
+      </c>
+      <c r="C29">
+        <v>0.5</v>
       </c>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B30">
         <v>0.5</v>
@@ -1168,38 +1170,26 @@
       <c r="C30">
         <v>0.5</v>
       </c>
-      <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="B31">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="C31">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>80</v>
-      </c>
-      <c r="B32">
-        <v>0.1</v>
-      </c>
-      <c r="C32">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>77</v>
-      </c>
-      <c r="B33" t="s">
-        <v>112</v>
-      </c>
-      <c r="E33" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="B32" t="s">
+        <v>85</v>
+      </c>
+      <c r="E32" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1214,918 +1204,919 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357397E0-3897-4AF9-B2FD-A8AFBCAC7335}">
   <dimension ref="A1:BZ27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>97</v>
+      <c r="A1" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>81</v>
+      <c r="B2" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4">
         <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <v>1</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="5">
         <v>1</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="5">
         <v>2</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="5">
         <v>3</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="5">
         <v>4</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="5">
         <v>5</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="5">
         <v>6</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="5">
         <v>7</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="5">
         <v>8</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="5">
         <v>9</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="5">
         <v>10</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="5">
         <v>11</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M5" s="5">
         <v>12</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N5" s="5">
         <v>13</v>
       </c>
-      <c r="O5" s="4">
+      <c r="O5" s="5">
         <v>14</v>
       </c>
-      <c r="P5" s="4">
+      <c r="P5" s="5">
         <v>15</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="Q5" s="5">
         <v>16</v>
       </c>
-      <c r="R5" s="4">
+      <c r="R5" s="5">
         <v>17</v>
       </c>
-      <c r="S5" s="4">
+      <c r="S5" s="5">
         <v>18</v>
       </c>
-      <c r="T5" s="4">
+      <c r="T5" s="5">
         <v>19</v>
       </c>
-      <c r="U5" s="4">
+      <c r="U5" s="5">
         <v>20</v>
       </c>
-      <c r="V5" s="4">
+      <c r="V5" s="5">
         <v>21</v>
       </c>
-      <c r="W5" s="4">
+      <c r="W5" s="5">
         <v>22</v>
       </c>
-      <c r="X5" s="4">
+      <c r="X5" s="5">
         <v>23</v>
       </c>
-      <c r="Y5" s="4">
+      <c r="Y5" s="5">
         <v>24</v>
       </c>
-      <c r="Z5" s="4">
+      <c r="Z5" s="5">
         <v>25</v>
       </c>
-      <c r="AA5" s="4">
+      <c r="AA5" s="5">
         <v>26</v>
       </c>
-      <c r="AB5" s="4">
+      <c r="AB5" s="5">
         <v>27</v>
       </c>
-      <c r="AC5" s="4">
+      <c r="AC5" s="5">
         <v>28</v>
       </c>
-      <c r="AD5" s="4">
+      <c r="AD5" s="5">
         <v>29</v>
       </c>
-      <c r="AE5" s="4">
+      <c r="AE5" s="5">
         <v>30</v>
       </c>
-      <c r="AF5" s="4">
+      <c r="AF5" s="5">
         <v>31</v>
       </c>
-      <c r="AG5" s="4">
+      <c r="AG5" s="5">
         <v>32</v>
       </c>
-      <c r="AH5" s="4">
+      <c r="AH5" s="5">
         <v>33</v>
       </c>
-      <c r="AI5" s="4">
+      <c r="AI5" s="5">
         <v>34</v>
       </c>
-      <c r="AJ5" s="4">
+      <c r="AJ5" s="5">
         <v>35</v>
       </c>
-      <c r="AK5" s="4">
+      <c r="AK5" s="5">
         <v>36</v>
       </c>
-      <c r="AL5" s="4">
+      <c r="AL5" s="5">
         <v>37</v>
       </c>
-      <c r="AM5" s="4">
+      <c r="AM5" s="5">
         <v>38</v>
       </c>
-      <c r="AN5" s="4">
+      <c r="AN5" s="5">
         <v>39</v>
       </c>
-      <c r="AO5" s="4">
+      <c r="AO5" s="5">
         <v>40</v>
       </c>
-      <c r="AP5" s="4">
+      <c r="AP5" s="5">
         <v>41</v>
       </c>
-      <c r="AQ5" s="4">
+      <c r="AQ5" s="5">
         <v>42</v>
       </c>
-      <c r="AR5" s="4">
+      <c r="AR5" s="5">
         <v>43</v>
       </c>
-      <c r="AS5" s="4">
+      <c r="AS5" s="5">
         <v>44</v>
       </c>
-      <c r="AT5" s="4">
+      <c r="AT5" s="5">
         <v>45</v>
       </c>
-      <c r="AU5" s="4">
+      <c r="AU5" s="5">
         <v>46</v>
       </c>
-      <c r="AV5" s="4">
+      <c r="AV5" s="5">
         <v>47</v>
       </c>
-      <c r="AW5" s="4">
+      <c r="AW5" s="5">
         <v>48</v>
       </c>
-      <c r="AX5" s="4">
+      <c r="AX5" s="5">
         <v>49</v>
       </c>
-      <c r="AY5" s="4">
+      <c r="AY5" s="5">
         <v>50</v>
       </c>
-      <c r="AZ5" s="4">
+      <c r="AZ5" s="5">
         <v>51</v>
       </c>
-      <c r="BA5" s="4">
+      <c r="BA5" s="5">
         <v>52</v>
       </c>
-      <c r="BB5" s="4">
+      <c r="BB5" s="5">
         <v>53</v>
       </c>
-      <c r="BC5" s="4">
+      <c r="BC5" s="5">
         <v>54</v>
       </c>
-      <c r="BD5" s="4">
+      <c r="BD5" s="5">
         <v>55</v>
       </c>
-      <c r="BE5" s="4">
+      <c r="BE5" s="5">
         <v>56</v>
       </c>
-      <c r="BF5" s="4">
+      <c r="BF5" s="5">
         <v>57</v>
       </c>
-      <c r="BG5" s="4">
+      <c r="BG5" s="5">
         <v>58</v>
       </c>
-      <c r="BH5" s="4">
+      <c r="BH5" s="5">
         <v>59</v>
       </c>
-      <c r="BI5" s="4">
+      <c r="BI5" s="5">
         <v>60</v>
       </c>
-      <c r="BJ5" s="4">
+      <c r="BJ5" s="5">
         <v>61</v>
       </c>
-      <c r="BK5" s="4">
+      <c r="BK5" s="5">
         <v>62</v>
       </c>
-      <c r="BL5" s="4">
+      <c r="BL5" s="5">
         <v>63</v>
       </c>
-      <c r="BM5" s="4">
+      <c r="BM5" s="5">
         <v>64</v>
       </c>
-      <c r="BN5" s="4">
+      <c r="BN5" s="5">
         <v>65</v>
       </c>
-      <c r="BO5" s="4">
+      <c r="BO5" s="5">
         <v>66</v>
       </c>
-      <c r="BP5" s="4">
+      <c r="BP5" s="5">
         <v>67</v>
       </c>
-      <c r="BQ5" s="4">
+      <c r="BQ5" s="5">
         <v>68</v>
       </c>
-      <c r="BR5" s="4">
+      <c r="BR5" s="5">
         <v>69</v>
       </c>
-      <c r="BS5" s="4">
+      <c r="BS5" s="5">
         <v>70</v>
       </c>
-      <c r="BT5" s="4">
+      <c r="BT5" s="5">
         <v>71</v>
       </c>
-      <c r="BU5" s="4">
+      <c r="BU5" s="5">
         <v>72</v>
       </c>
-      <c r="BV5" s="4">
+      <c r="BV5" s="5">
         <v>73</v>
       </c>
-      <c r="BW5" s="4">
+      <c r="BW5" s="5">
         <v>74</v>
       </c>
-      <c r="BX5" s="4">
+      <c r="BX5" s="5">
         <v>75</v>
       </c>
-      <c r="BY5" s="4">
+      <c r="BY5" s="5">
         <v>76</v>
       </c>
-      <c r="BZ5" s="4">
+      <c r="BZ5" s="5">
         <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="6">
         <v>1.4189701897018967E-2</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="6">
         <v>0</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="6">
         <v>2.1284552845528448E-2</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="6">
         <v>2.1284552845528448E-2</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="6">
         <v>2.1284552845528448E-2</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="6">
         <v>2.1284552845528448E-2</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="6">
         <v>3.5474254742547416E-2</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="6">
         <v>4.9663956639566395E-2</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="6">
         <v>4.9663956639566395E-2</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="6">
         <v>6.3853658536585339E-2</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="6">
         <v>7.0948509485094832E-2</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="6">
         <v>9.2233062330623283E-2</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="6">
         <v>0.12770731707317068</v>
       </c>
-      <c r="O6" s="5">
+      <c r="O6" s="6">
         <v>9.2233062330623283E-2</v>
       </c>
-      <c r="P6" s="5">
+      <c r="P6" s="6">
         <v>9.2233062330623283E-2</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="Q6" s="6">
         <v>0.15608672086720862</v>
       </c>
-      <c r="R6" s="5">
+      <c r="R6" s="6">
         <v>0.12770731707317068</v>
       </c>
-      <c r="S6" s="5">
+      <c r="S6" s="6">
         <v>0.17027642276422758</v>
       </c>
-      <c r="T6" s="5">
+      <c r="T6" s="6">
         <v>0.13480216802168019</v>
       </c>
-      <c r="U6" s="5">
+      <c r="U6" s="6">
         <v>0.14899186991869914</v>
       </c>
-      <c r="V6" s="5">
+      <c r="V6" s="6">
         <v>0.19156097560975605</v>
       </c>
-      <c r="W6" s="5">
+      <c r="W6" s="6">
         <v>0.16318157181571813</v>
       </c>
-      <c r="X6" s="5">
+      <c r="X6" s="6">
         <v>0.18446612466124657</v>
       </c>
-      <c r="Y6" s="5">
+      <c r="Y6" s="6">
         <v>0.24122493224932245</v>
       </c>
-      <c r="Z6" s="5">
+      <c r="Z6" s="6">
         <v>0.19156097560975605</v>
       </c>
-      <c r="AA6" s="5">
+      <c r="AA6" s="6">
         <v>0.30507859078590777</v>
       </c>
-      <c r="AB6" s="5">
+      <c r="AB6" s="6">
         <v>0.25541463414634136</v>
       </c>
-      <c r="AC6" s="5">
+      <c r="AC6" s="6">
         <v>0.21284552845528448</v>
       </c>
-      <c r="AD6" s="5">
+      <c r="AD6" s="6">
         <v>0.39731165311653116</v>
       </c>
-      <c r="AE6" s="5">
+      <c r="AE6" s="6">
         <v>0.28379403794037933</v>
       </c>
-      <c r="AF6" s="5">
+      <c r="AF6" s="6">
         <v>0.31926829268292678</v>
       </c>
-      <c r="AG6" s="5">
+      <c r="AG6" s="6">
         <v>0.16318157181571813</v>
       </c>
-      <c r="AH6" s="5">
+      <c r="AH6" s="6">
         <v>0.31217344173441725</v>
       </c>
-      <c r="AI6" s="5">
+      <c r="AI6" s="6">
         <v>0.15608672086720862</v>
       </c>
-      <c r="AJ6" s="5">
+      <c r="AJ6" s="6">
         <v>0.14899186991869914</v>
       </c>
-      <c r="AK6" s="5">
+      <c r="AK6" s="6">
         <v>0.14899186991869914</v>
       </c>
-      <c r="AL6" s="5">
+      <c r="AL6" s="6">
         <v>0.14189701897018966</v>
       </c>
-      <c r="AM6" s="5">
+      <c r="AM6" s="6">
         <v>0.205750677506775</v>
       </c>
-      <c r="AN6" s="5">
+      <c r="AN6" s="6">
         <v>9.932791327913279E-2</v>
       </c>
-      <c r="AO6" s="5">
+      <c r="AO6" s="6">
         <v>0.14189701897018966</v>
       </c>
-      <c r="AP6" s="5">
+      <c r="AP6" s="6">
         <v>0.13480216802168019</v>
       </c>
-      <c r="AQ6" s="5">
+      <c r="AQ6" s="6">
         <v>0.16318157181571813</v>
       </c>
-      <c r="AR6" s="5">
+      <c r="AR6" s="6">
         <v>0.11351761517615173</v>
       </c>
-      <c r="AS6" s="5">
+      <c r="AS6" s="6">
         <v>9.932791327913279E-2</v>
       </c>
-      <c r="AT6" s="5">
+      <c r="AT6" s="6">
         <v>0.10642276422764224</v>
       </c>
-      <c r="AU6" s="5">
+      <c r="AU6" s="6">
         <v>8.513821138211379E-2</v>
       </c>
-      <c r="AV6" s="5">
+      <c r="AV6" s="6">
         <v>0.10642276422764224</v>
       </c>
-      <c r="AW6" s="5">
+      <c r="AW6" s="6">
         <v>7.0948509485094832E-2</v>
       </c>
-      <c r="AX6" s="5">
+      <c r="AX6" s="6">
         <v>0.14899186991869914</v>
       </c>
-      <c r="AY6" s="5">
+      <c r="AY6" s="6">
         <v>0.13480216802168019</v>
       </c>
-      <c r="AZ6" s="5">
+      <c r="AZ6" s="6">
         <v>0.11351761517615173</v>
       </c>
-      <c r="BA6" s="5">
+      <c r="BA6" s="6">
         <v>0.10642276422764224</v>
       </c>
-      <c r="BB6" s="5">
+      <c r="BB6" s="6">
         <v>0.12061246612466123</v>
       </c>
-      <c r="BC6" s="5">
+      <c r="BC6" s="6">
         <v>0.14189701897018966</v>
       </c>
-      <c r="BD6" s="5">
+      <c r="BD6" s="6">
         <v>6.3853658536585339E-2</v>
       </c>
-      <c r="BE6" s="5">
+      <c r="BE6" s="6">
         <v>7.0948509485094832E-2</v>
       </c>
-      <c r="BF6" s="5">
+      <c r="BF6" s="6">
         <v>9.2233062330623283E-2</v>
       </c>
-      <c r="BG6" s="5">
+      <c r="BG6" s="6">
         <v>8.513821138211379E-2</v>
       </c>
-      <c r="BH6" s="5">
+      <c r="BH6" s="6">
         <v>9.2233062330623283E-2</v>
       </c>
-      <c r="BI6" s="5">
+      <c r="BI6" s="6">
         <v>0.19156097560975605</v>
       </c>
-      <c r="BJ6" s="5">
+      <c r="BJ6" s="6">
         <v>0.21994037940379399</v>
       </c>
-      <c r="BK6" s="5">
+      <c r="BK6" s="6">
         <v>0.36183739837398371</v>
       </c>
-      <c r="BL6" s="5">
+      <c r="BL6" s="6">
         <v>0.56049322493224918</v>
       </c>
-      <c r="BM6" s="5">
+      <c r="BM6" s="6">
         <v>0.4682601626016259</v>
       </c>
-      <c r="BN6" s="5">
+      <c r="BN6" s="6">
         <v>0.43278590785907844</v>
       </c>
-      <c r="BO6" s="5">
+      <c r="BO6" s="6">
         <v>0.26960433604336037</v>
       </c>
-      <c r="BP6" s="5">
+      <c r="BP6" s="6">
         <v>0.34055284552845516</v>
       </c>
-      <c r="BQ6" s="5">
+      <c r="BQ6" s="6">
         <v>0.28379403794037933</v>
       </c>
-      <c r="BR6" s="5">
+      <c r="BR6" s="6">
         <v>0.27669918699186985</v>
       </c>
-      <c r="BS6" s="5">
+      <c r="BS6" s="6">
         <v>0.27669918699186985</v>
       </c>
-      <c r="BT6" s="5">
+      <c r="BT6" s="6">
         <v>0.29088888888888881</v>
       </c>
-      <c r="BU6" s="5">
+      <c r="BU6" s="6">
         <v>0.29798373983739829</v>
       </c>
-      <c r="BV6" s="5">
+      <c r="BV6" s="6">
         <v>0.27669918699186985</v>
       </c>
-      <c r="BW6" s="5">
+      <c r="BW6" s="6">
         <v>0.28379403794037933</v>
       </c>
-      <c r="BX6" s="5">
+      <c r="BX6" s="6">
         <v>0.14899186991869914</v>
       </c>
-      <c r="BY6" s="5">
+      <c r="BY6" s="6">
         <v>0.14899186991869914</v>
       </c>
-      <c r="BZ6" s="5">
+      <c r="BZ6" s="6">
         <v>0.13480216802168019</v>
       </c>
     </row>
     <row r="7" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="6">
         <v>3.3387533875338743E-2</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="6">
         <v>0</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="6">
         <v>5.0081300813008114E-2</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="6">
         <v>5.0081300813008114E-2</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="6">
         <v>5.0081300813008114E-2</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="6">
         <v>5.0081300813008114E-2</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="6">
         <v>8.3468834688346871E-2</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="6">
         <v>0.11685636856368563</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="6">
         <v>0.11685636856368563</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="6">
         <v>0.15024390243902433</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="6">
         <v>0.16693766937669374</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="6">
         <v>0.21701897018970184</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="6">
         <v>0.30048780487804866</v>
       </c>
-      <c r="O7" s="5">
+      <c r="O7" s="6">
         <v>0.21701897018970184</v>
       </c>
-      <c r="P7" s="5">
+      <c r="P7" s="6">
         <v>0.21701897018970184</v>
       </c>
-      <c r="Q7" s="5">
+      <c r="Q7" s="6">
         <v>0.36726287262872614</v>
       </c>
-      <c r="R7" s="5">
+      <c r="R7" s="6">
         <v>0.30048780487804866</v>
       </c>
-      <c r="S7" s="5">
+      <c r="S7" s="6">
         <v>0.40065040650406492</v>
       </c>
-      <c r="T7" s="5">
+      <c r="T7" s="6">
         <v>0.31718157181571804</v>
       </c>
-      <c r="U7" s="5">
+      <c r="U7" s="6">
         <v>0.35056910569105681</v>
       </c>
-      <c r="V7" s="5">
+      <c r="V7" s="6">
         <v>0.45073170731707307</v>
       </c>
-      <c r="W7" s="5">
+      <c r="W7" s="6">
         <v>0.38395663956639559</v>
       </c>
-      <c r="X7" s="5">
+      <c r="X7" s="6">
         <v>0.43403794037940369</v>
       </c>
-      <c r="Y7" s="5">
+      <c r="Y7" s="6">
         <v>0.56758807588075866</v>
       </c>
-      <c r="Z7" s="5">
+      <c r="Z7" s="6">
         <v>0.45073170731707307</v>
       </c>
-      <c r="AA7" s="5">
+      <c r="AA7" s="6">
         <v>0.71783197831978296</v>
       </c>
-      <c r="AB7" s="5">
+      <c r="AB7" s="6">
         <v>0.60097560975609732</v>
       </c>
-      <c r="AC7" s="5">
+      <c r="AC7" s="6">
         <v>0.50081300813008112</v>
       </c>
-      <c r="AD7" s="5">
+      <c r="AD7" s="6">
         <v>0.93485094850948502</v>
       </c>
-      <c r="AE7" s="5">
+      <c r="AE7" s="6">
         <v>0.66775067750677497</v>
       </c>
-      <c r="AF7" s="5">
+      <c r="AF7" s="6">
         <v>0.75121951219512173</v>
       </c>
-      <c r="AG7" s="5">
+      <c r="AG7" s="6">
         <v>0.38395663956639559</v>
       </c>
-      <c r="AH7" s="5">
+      <c r="AH7" s="6">
         <v>0.73452574525745229</v>
       </c>
-      <c r="AI7" s="5">
+      <c r="AI7" s="6">
         <v>0.36726287262872614</v>
       </c>
-      <c r="AJ7" s="5">
+      <c r="AJ7" s="6">
         <v>0.35056910569105681</v>
       </c>
-      <c r="AK7" s="5">
+      <c r="AK7" s="6">
         <v>0.35056910569105681</v>
       </c>
-      <c r="AL7" s="5">
+      <c r="AL7" s="6">
         <v>0.33387533875338749</v>
       </c>
-      <c r="AM7" s="5">
+      <c r="AM7" s="6">
         <v>0.48411924119241179</v>
       </c>
-      <c r="AN7" s="5">
+      <c r="AN7" s="6">
         <v>0.23371273712737126</v>
       </c>
-      <c r="AO7" s="5">
+      <c r="AO7" s="6">
         <v>0.33387533875338749</v>
       </c>
-      <c r="AP7" s="5">
+      <c r="AP7" s="6">
         <v>0.31718157181571804</v>
       </c>
-      <c r="AQ7" s="5">
+      <c r="AQ7" s="6">
         <v>0.38395663956639559</v>
       </c>
-      <c r="AR7" s="5">
+      <c r="AR7" s="6">
         <v>0.26710027100270994</v>
       </c>
-      <c r="AS7" s="5">
+      <c r="AS7" s="6">
         <v>0.23371273712737126</v>
       </c>
-      <c r="AT7" s="5">
+      <c r="AT7" s="6">
         <v>0.25040650406504056</v>
       </c>
-      <c r="AU7" s="5">
+      <c r="AU7" s="6">
         <v>0.20032520325203246</v>
       </c>
-      <c r="AV7" s="5">
+      <c r="AV7" s="6">
         <v>0.25040650406504056</v>
       </c>
-      <c r="AW7" s="5">
+      <c r="AW7" s="6">
         <v>0.16693766937669374</v>
       </c>
-      <c r="AX7" s="5">
+      <c r="AX7" s="6">
         <v>0.35056910569105681</v>
       </c>
-      <c r="AY7" s="5">
+      <c r="AY7" s="6">
         <v>0.31718157181571804</v>
       </c>
-      <c r="AZ7" s="5">
+      <c r="AZ7" s="6">
         <v>0.26710027100270994</v>
       </c>
-      <c r="BA7" s="5">
+      <c r="BA7" s="6">
         <v>0.25040650406504056</v>
       </c>
-      <c r="BB7" s="5">
+      <c r="BB7" s="6">
         <v>0.28379403794037933</v>
       </c>
-      <c r="BC7" s="5">
+      <c r="BC7" s="6">
         <v>0.33387533875338749</v>
       </c>
-      <c r="BD7" s="5">
+      <c r="BD7" s="6">
         <v>0.15024390243902433</v>
       </c>
-      <c r="BE7" s="5">
+      <c r="BE7" s="6">
         <v>0.16693766937669374</v>
       </c>
-      <c r="BF7" s="5">
+      <c r="BF7" s="6">
         <v>0.21701897018970184</v>
       </c>
-      <c r="BG7" s="5">
+      <c r="BG7" s="6">
         <v>0.20032520325203246</v>
       </c>
-      <c r="BH7" s="5">
+      <c r="BH7" s="6">
         <v>0.21701897018970184</v>
       </c>
-      <c r="BI7" s="5">
+      <c r="BI7" s="6">
         <v>0.45073170731707307</v>
       </c>
-      <c r="BJ7" s="5">
+      <c r="BJ7" s="6">
         <v>0.51750677506775056</v>
       </c>
-      <c r="BK7" s="5">
+      <c r="BK7" s="6">
         <v>0.85138211382113804</v>
       </c>
-      <c r="BL7" s="5">
+      <c r="BL7" s="6">
         <v>1.3188075880758805</v>
       </c>
-      <c r="BM7" s="5">
+      <c r="BM7" s="6">
         <v>1.1017886178861784</v>
       </c>
-      <c r="BN7" s="5">
+      <c r="BN7" s="6">
         <v>1.0183197831978317</v>
       </c>
-      <c r="BO7" s="5">
+      <c r="BO7" s="6">
         <v>0.63436314363143609</v>
       </c>
-      <c r="BP7" s="5">
+      <c r="BP7" s="6">
         <v>0.80130081300812983</v>
       </c>
-      <c r="BQ7" s="5">
+      <c r="BQ7" s="6">
         <v>0.66775067750677497</v>
       </c>
-      <c r="BR7" s="5">
+      <c r="BR7" s="6">
         <v>0.65105691056910553</v>
       </c>
-      <c r="BS7" s="5">
+      <c r="BS7" s="6">
         <v>0.65105691056910553</v>
       </c>
-      <c r="BT7" s="5">
+      <c r="BT7" s="6">
         <v>0.68444444444444419</v>
       </c>
-      <c r="BU7" s="5">
+      <c r="BU7" s="6">
         <v>0.70113821138211363</v>
       </c>
-      <c r="BV7" s="5">
+      <c r="BV7" s="6">
         <v>0.65105691056910553</v>
       </c>
-      <c r="BW7" s="5">
+      <c r="BW7" s="6">
         <v>0.66775067750677497</v>
       </c>
-      <c r="BX7" s="5">
+      <c r="BX7" s="6">
         <v>0.35056910569105681</v>
       </c>
-      <c r="BY7" s="5">
+      <c r="BY7" s="6">
         <v>0.35056910569105681</v>
       </c>
-      <c r="BZ7" s="5">
+      <c r="BZ7" s="6">
         <v>0.31718157181571804</v>
       </c>
     </row>
     <row r="8" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B8">
+      <c r="A8" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="4">
         <v>0</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="4">
         <v>0</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="4">
         <v>0.1</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="4">
         <v>0.3</v>
       </c>
     </row>
     <row r="11" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="4">
         <v>15</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="4">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="4">
         <v>35</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="4">
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="4">
         <v>1</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B14" t="b">
+      <c r="B14" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>85</v>
-      </c>
-      <c r="B15">
+      <c r="A15" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="4">
         <v>20</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="4">
         <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>86</v>
-      </c>
-      <c r="B16">
+      <c r="A16" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="4">
         <v>40</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="4">
         <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>87</v>
-      </c>
-      <c r="B17">
+      <c r="A17" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="4">
         <v>1</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>88</v>
-      </c>
-      <c r="B18">
+      <c r="A18" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="4">
         <v>0</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>89</v>
-      </c>
-      <c r="B27">
+      <c r="A27" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="4">
         <v>2016</v>
       </c>
     </row>
@@ -2136,10 +2127,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D84B13DB-B1C4-4EAE-94F6-E80E232D9006}">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2150,7 +2141,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2158,7 +2149,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2226,110 +2217,107 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>50</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="B10">
-        <v>0.1</v>
-      </c>
-      <c r="C10">
-        <v>0.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>0.1</v>
+      </c>
+      <c r="C11">
+        <v>0.3</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="B12">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="C12">
-        <v>0.3</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B13">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>90</v>
       </c>
       <c r="B15">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="B16">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>92</v>
       </c>
       <c r="B17">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="B19">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="B20">
         <v>0.05</v>
@@ -2337,39 +2325,39 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="B21">
-        <v>0.05</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>97</v>
       </c>
       <c r="B22">
-        <v>0.4</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="B23">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>99</v>
       </c>
       <c r="B24">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="B25">
         <v>0.2</v>
@@ -2377,111 +2365,48 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="B26">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="B27">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="B28">
-        <v>0.25</v>
+        <v>0.05</v>
+      </c>
+      <c r="C28">
+        <v>0.1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>102</v>
       </c>
       <c r="B29">
-        <v>0.05</v>
-      </c>
-      <c r="C29">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="B30">
+        <v>0.1</v>
+      </c>
+      <c r="C30">
         <v>0.2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>66</v>
-      </c>
-      <c r="B31">
-        <v>0.1</v>
-      </c>
-      <c r="C31">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>92</v>
-      </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>93</v>
-      </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>94</v>
-      </c>
-      <c r="B34">
-        <v>0</v>
-      </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>95</v>
-      </c>
-      <c r="B35">
-        <v>0</v>
-      </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>96</v>
-      </c>
-      <c r="B36">
-        <v>0</v>
-      </c>
-      <c r="C36">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2494,90 +2419,91 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>97</v>
+      <c r="A1" s="7" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>83</v>
+      <c r="B2" s="7" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3">
+      <c r="A3" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="7">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="7">
         <v>1.2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4">
+      <c r="A4" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="7">
         <v>0.05</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="7">
         <v>0.1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5">
+      <c r="A5" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="7">
         <v>1</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="7">
         <v>1.2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B6">
+      <c r="A6" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="7">
         <v>0.05</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="7">
         <v>0.1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7">
+      <c r="A7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="7">
         <v>1</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B8">
+      <c r="A8" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="7">
         <v>0.05</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="7">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix typo in Excel
</commit_message>
<xml_diff>
--- a/inst/Example_Chile_Hake.xlsx
+++ b/inst/Example_Chile_Hake.xlsx
@@ -175,9 +175,6 @@
     <t>isRel</t>
   </si>
   <si>
-    <t>LenMcv</t>
-  </si>
-  <si>
     <t>Cobs</t>
   </si>
   <si>
@@ -362,13 +359,16 @@
   </si>
   <si>
     <t>TAEFrac</t>
+  </si>
+  <si>
+    <t>LenMbiascv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -384,6 +384,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -433,7 +440,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -444,6 +451,7 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -784,7 +792,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -792,12 +800,12 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3">
         <v>200</v>
@@ -805,7 +813,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4">
         <v>50</v>
@@ -813,7 +821,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -821,35 +829,35 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6">
         <v>0.5</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B7">
         <v>0.8</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -874,13 +882,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" t="s">
         <v>83</v>
-      </c>
-      <c r="C1" t="s">
-        <v>84</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -890,7 +898,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -922,12 +930,12 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1001,12 +1009,12 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1044,7 +1052,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B19">
         <v>0.1</v>
@@ -1173,7 +1181,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B31">
         <v>0.1</v>
@@ -1184,10 +1192,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E32" s="1"/>
     </row>
@@ -1216,7 +1224,7 @@
   <sheetData>
     <row r="1" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:78" x14ac:dyDescent="0.25">
@@ -1224,7 +1232,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:78" x14ac:dyDescent="0.25">
@@ -1956,7 +1964,7 @@
     </row>
     <row r="8" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B8" s="4">
         <v>0</v>
@@ -2030,7 +2038,7 @@
     </row>
     <row r="15" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B15" s="4">
         <v>20</v>
@@ -2041,7 +2049,7 @@
     </row>
     <row r="16" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" s="4">
         <v>40</v>
@@ -2052,7 +2060,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B17" s="4">
         <v>1</v>
@@ -2063,7 +2071,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B18" s="4">
         <v>0</v>
@@ -2114,7 +2122,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B27" s="4">
         <v>2016</v>
@@ -2130,282 +2138,283 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>71</v>
+      <c r="A1" s="8" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>62</v>
+      <c r="B2" s="8" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="C3" s="8">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B3">
+      <c r="B4" s="8">
         <v>0.1</v>
       </c>
-      <c r="C3">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="8">
+        <v>250</v>
+      </c>
+      <c r="C5" s="8">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="8">
+        <v>50</v>
+      </c>
+      <c r="C6" s="8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="8">
+        <v>5000</v>
+      </c>
+      <c r="C7" s="8">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="8">
+        <v>50</v>
+      </c>
+      <c r="C8" s="8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="C9" s="8">
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="8">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5">
-        <v>250</v>
-      </c>
-      <c r="C5">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6">
+      <c r="C11" s="8">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="C12" s="8">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="8">
+        <v>1</v>
+      </c>
+      <c r="C13" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="8">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="8">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" s="8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19" s="8">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" s="8">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" s="8">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" s="8">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="8">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" s="8">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25" s="8">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B26" s="8">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C6">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7">
-        <v>5000</v>
-      </c>
-      <c r="C7">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8">
-        <v>50</v>
-      </c>
-      <c r="C8">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9">
+      <c r="B27" s="8">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="C28" s="8">
         <v>0.1</v>
       </c>
-      <c r="C9">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>89</v>
-      </c>
-      <c r="B11">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="8">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B30" s="8">
         <v>0.1</v>
       </c>
-      <c r="C11">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>86</v>
-      </c>
-      <c r="B12">
-        <v>0.8</v>
-      </c>
-      <c r="C12">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>90</v>
-      </c>
-      <c r="B15">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>91</v>
-      </c>
-      <c r="B16">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>92</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>93</v>
-      </c>
-      <c r="B18">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>94</v>
-      </c>
-      <c r="B19">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>95</v>
-      </c>
-      <c r="B20">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>96</v>
-      </c>
-      <c r="B21">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>97</v>
-      </c>
-      <c r="B22">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>98</v>
-      </c>
-      <c r="B23">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B24">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>100</v>
-      </c>
-      <c r="B25">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>101</v>
-      </c>
-      <c r="B26">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>88</v>
-      </c>
-      <c r="B28">
-        <v>0.05</v>
-      </c>
-      <c r="C28">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>102</v>
-      </c>
-      <c r="B29">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>103</v>
-      </c>
-      <c r="B30">
-        <v>0.1</v>
-      </c>
-      <c r="C30">
+      <c r="C30" s="8">
         <v>0.2</v>
       </c>
     </row>
@@ -2430,7 +2439,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2438,12 +2447,12 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="7">
         <v>1</v>
@@ -2454,7 +2463,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="7">
         <v>0.05</v>
@@ -2465,7 +2474,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" s="7">
         <v>1</v>
@@ -2476,7 +2485,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B6" s="7">
         <v>0.05</v>
@@ -2487,7 +2496,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="7">
         <v>1</v>
@@ -2498,7 +2507,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" s="7">
         <v>0.05</v>

</xml_diff>

<commit_message>
fix more typos in Rmd!
</commit_message>
<xml_diff>
--- a/inst/Example_Chile_Hake.xlsx
+++ b/inst/Example_Chile_Hake.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8970" tabRatio="736" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8970" tabRatio="736" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="OM" sheetId="13" r:id="rId1"/>
-    <sheet name="Stock" sheetId="1" r:id="rId2"/>
-    <sheet name="Fleet" sheetId="15" r:id="rId3"/>
-    <sheet name="Obs" sheetId="16" r:id="rId4"/>
-    <sheet name="Imp" sheetId="17" r:id="rId5"/>
+    <sheet name="Stock" sheetId="1" r:id="rId1"/>
+    <sheet name="Fleet" sheetId="15" r:id="rId2"/>
+    <sheet name="Obs" sheetId="16" r:id="rId3"/>
+    <sheet name="Imp" sheetId="17" r:id="rId4"/>
+    <sheet name="OM" sheetId="13" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="a50mat">#REF!</definedName>
@@ -777,99 +777,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BAE3F1A-90BF-4F3A-B6A0-6C07DD5D0F91}">
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B6">
-        <v>0.5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7">
-        <v>0.8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
@@ -1208,7 +1119,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357397E0-3897-4AF9-B2FD-A8AFBCAC7335}">
   <dimension ref="A1:BZ27"/>
   <sheetViews>
@@ -2133,11 +2044,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D84B13DB-B1C4-4EAE-94F6-E80E232D9006}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -2423,7 +2334,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55CE1B81-1FA9-4A2B-B1E2-B75843FD27F8}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -2519,4 +2430,93 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BAE3F1A-90BF-4F3A-B6A0-6C07DD5D0F91}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6">
+        <v>0.5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7">
+        <v>0.8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>